<commit_message>
test: Added tests to verify a program can have multiple agencies
</commit_message>
<xml_diff>
--- a/epic_app/tests/test_data/xlsx/agency_data.xlsx
+++ b/epic_app/tests/test_data/xlsx/agency_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-Tool\backend\epic_app\tests\test_data\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\EPIC-api\epic_app\tests\test_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E5D0EA-23E3-42DE-9DBB-7D9DA9D9AC32}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308B40C6-0321-4791-93F6-A5121BCA5FFB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3732" windowWidth="17280" windowHeight="9216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agency_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="49">
   <si>
     <t>Agency</t>
   </si>
@@ -1022,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:XFD83"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1493,13 +1493,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1507,7 +1504,10 @@
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1515,7 +1515,7 @@
         <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1523,7 +1523,7 @@
         <v>36</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1531,7 +1531,7 @@
         <v>36</v>
       </c>
       <c r="B52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1539,7 +1539,7 @@
         <v>36</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1547,7 +1547,7 @@
         <v>36</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1555,10 +1555,7 @@
         <v>36</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
-      </c>
-      <c r="C55" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1566,7 +1563,7 @@
         <v>36</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -1577,7 +1574,10 @@
         <v>36</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1585,10 +1585,7 @@
         <v>36</v>
       </c>
       <c r="B58" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1596,7 +1593,7 @@
         <v>36</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1604,10 +1601,13 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B60" t="s">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1615,7 +1615,7 @@
         <v>41</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1623,7 +1623,7 @@
         <v>41</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1631,7 +1631,7 @@
         <v>41</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1639,7 +1639,7 @@
         <v>41</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1647,7 +1647,7 @@
         <v>41</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1655,10 +1655,7 @@
         <v>41</v>
       </c>
       <c r="B66" t="s">
-        <v>42</v>
-      </c>
-      <c r="C66" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1666,7 +1663,7 @@
         <v>41</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
@@ -1677,7 +1674,7 @@
         <v>41</v>
       </c>
       <c r="B68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -1688,7 +1685,7 @@
         <v>41</v>
       </c>
       <c r="B69" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
@@ -1696,10 +1693,13 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1707,7 +1707,7 @@
         <v>45</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -1715,7 +1715,7 @@
         <v>45</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1723,7 +1723,7 @@
         <v>45</v>
       </c>
       <c r="B73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -1731,7 +1731,7 @@
         <v>45</v>
       </c>
       <c r="B74" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1739,7 +1739,7 @@
         <v>45</v>
       </c>
       <c r="B75" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1747,18 +1747,18 @@
         <v>45</v>
       </c>
       <c r="B76" t="s">
-        <v>40</v>
-      </c>
-      <c r="C76" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B77" t="s">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -1766,7 +1766,7 @@
         <v>46</v>
       </c>
       <c r="B78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -1774,7 +1774,7 @@
         <v>46</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -1782,7 +1782,7 @@
         <v>46</v>
       </c>
       <c r="B80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1790,7 +1790,7 @@
         <v>46</v>
       </c>
       <c r="B81" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1798,7 +1798,7 @@
         <v>46</v>
       </c>
       <c r="B82" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1806,6 +1806,14 @@
         <v>46</v>
       </c>
       <c r="B83" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1816,12 +1824,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2054,15 +2059,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2087,10 +2096,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BBC2A99-7D7D-4036-A3B4-ADBCCCAD22CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61E416E2-4A6A-4C1B-B794-2BED7D3C2983}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>